<commit_message>
Updated demo to include multiline non-wrapped text
</commit_message>
<xml_diff>
--- a/ClosedXmlTest/template.xlsx
+++ b/ClosedXmlTest/template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\WEX\git\ClosedXmlDemo\ClosedXmlTest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7132C7E-A013-4D6C-B1DD-70CA2DCB75EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9AF6375-6D55-4A43-9A2D-FFFC320A5965}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{08197496-0D4F-4CC8-941F-905E26816427}"/>
   </bookViews>
@@ -16,8 +16,8 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="DataItems">Sheet1!$A$2:$C$3</definedName>
-    <definedName name="ReportHeaders">Sheet1!$B$1:$C$1</definedName>
+    <definedName name="DataItems">Sheet1!$A$2:$D$3</definedName>
+    <definedName name="ReportHeaders">Sheet1!$B$1:$D$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>{{item.Id}}</t>
   </si>
@@ -46,10 +46,16 @@
     <t>ID</t>
   </si>
   <si>
-    <t>Text</t>
-  </si>
-  <si>
-    <t>{{item.Text}}</t>
+    <t>WrappedText</t>
+  </si>
+  <si>
+    <t>MultilineText</t>
+  </si>
+  <si>
+    <t>{{item.MultilineText}}</t>
+  </si>
+  <si>
+    <t>{{item.WrappedText}}</t>
   </si>
 </sst>
 </file>
@@ -407,31 +413,38 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5621B4F8-6704-4BC9-B53E-F4096977DE46}">
-  <dimension ref="B1:C2"/>
+  <dimension ref="B1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:C2"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="25.28515625" customWidth="1"/>
+    <col min="4" max="4" width="18.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>3</v>
+        <v>5</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>